<commit_message>
Schema - clean-up and test DACPAC
Which didn't work - can't get to compile
</commit_message>
<xml_diff>
--- a/INJECT_DATA/SCMMembers.xlsx
+++ b/INJECT_DATA/SCMMembers.xlsx
@@ -1836,6 +1836,11 @@
       <c r="G38" t="b">
         <v>0</v>
       </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I38">
         <v>2</v>
       </c>
@@ -1925,6 +1930,11 @@
       <c r="G40" t="b">
         <v>0</v>
       </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I40">
         <v>2</v>
       </c>
@@ -2484,6 +2494,11 @@
       <c r="G52" t="b">
         <v>0</v>
       </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I52">
         <v>1</v>
       </c>
@@ -2526,6 +2541,11 @@
       <c r="G53" t="b">
         <v>0</v>
       </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I53">
         <v>2</v>
       </c>
@@ -2568,6 +2588,11 @@
       <c r="G54" t="b">
         <v>0</v>
       </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I54">
         <v>2</v>
       </c>
@@ -2704,6 +2729,11 @@
       <c r="G57" t="b">
         <v>0</v>
       </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I57">
         <v>1</v>
       </c>
@@ -3075,6 +3105,11 @@
       <c r="G65" t="b">
         <v>0</v>
       </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I65">
         <v>1</v>
       </c>
@@ -3305,6 +3340,11 @@
       <c r="G70" t="b">
         <v>0</v>
       </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I70">
         <v>2</v>
       </c>
@@ -3676,6 +3716,11 @@
       <c r="G78" t="b">
         <v>0</v>
       </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I78">
         <v>2</v>
       </c>
@@ -3718,6 +3763,11 @@
       <c r="G79" t="b">
         <v>0</v>
       </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I79">
         <v>2</v>
       </c>
@@ -3760,6 +3810,11 @@
       <c r="G80" t="b">
         <v>0</v>
       </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I80">
         <v>2</v>
       </c>
@@ -3802,6 +3857,11 @@
       <c r="G81" t="b">
         <v>0</v>
       </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I81">
         <v>2</v>
       </c>
@@ -3844,6 +3904,11 @@
       <c r="G82" t="b">
         <v>0</v>
       </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I82">
         <v>2</v>
       </c>
@@ -3883,6 +3948,11 @@
       <c r="G83" t="b">
         <v>0</v>
       </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I83">
         <v>2</v>
       </c>
@@ -3925,6 +3995,11 @@
       <c r="G84" t="b">
         <v>0</v>
       </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I84">
         <v>2</v>
       </c>
@@ -3967,6 +4042,11 @@
       <c r="G85" t="b">
         <v>0</v>
       </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I85">
         <v>1</v>
       </c>
@@ -4009,6 +4089,11 @@
       <c r="G86" t="b">
         <v>0</v>
       </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I86">
         <v>1</v>
       </c>
@@ -4051,6 +4136,11 @@
       <c r="G87" t="b">
         <v>0</v>
       </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I87">
         <v>2</v>
       </c>
@@ -4140,6 +4230,11 @@
       <c r="G89" t="b">
         <v>0</v>
       </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I89">
         <v>2</v>
       </c>
@@ -4182,6 +4277,11 @@
       <c r="G90" t="b">
         <v>0</v>
       </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I90">
         <v>2</v>
       </c>
@@ -4224,6 +4324,11 @@
       <c r="G91" t="b">
         <v>0</v>
       </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I91">
         <v>1</v>
       </c>
@@ -4310,6 +4415,11 @@
       <c r="G93" t="b">
         <v>0</v>
       </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I93">
         <v>1</v>
       </c>
@@ -4352,6 +4462,11 @@
       <c r="G94" t="b">
         <v>0</v>
       </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I94">
         <v>1</v>
       </c>
@@ -4394,6 +4509,11 @@
       <c r="G95" t="b">
         <v>0</v>
       </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I95">
         <v>1</v>
       </c>
@@ -4483,6 +4603,11 @@
       <c r="G97" t="b">
         <v>0</v>
       </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I97">
         <v>1</v>
       </c>
@@ -4619,6 +4744,11 @@
       <c r="G100" t="b">
         <v>0</v>
       </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="I100">
         <v>1</v>
       </c>

</xml_diff>